<commit_message>
Updated all important files
</commit_message>
<xml_diff>
--- a/Project Datasheet.xlsx
+++ b/Project Datasheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexn\OneDrive\Documents\Fundamentals of Data Science\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexn\OneDrive\Documents\Fundamentals of Data Science\Final Project - Starbucks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9FC826-54A3-4D6F-B392-81F6E05D7B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6779D1F-3401-4D0B-84A3-705F0594DF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{DCF5F147-EA5E-49E6-ACFB-A44835264122}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{DCF5F147-EA5E-49E6-ACFB-A44835264122}"/>
   </bookViews>
   <sheets>
     <sheet name="Drink Prices" sheetId="1" r:id="rId1"/>
@@ -567,27 +567,27 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -633,7 +633,7 @@
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -674,7 +674,7 @@
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -700,7 +700,7 @@
       <c r="P3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -726,7 +726,7 @@
       <c r="P4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -752,7 +752,7 @@
       <c r="P5" s="3"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -778,7 +778,7 @@
       <c r="P6" s="3"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -804,7 +804,7 @@
       <c r="P7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -830,7 +830,7 @@
       <c r="P8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -856,7 +856,7 @@
       <c r="P9" s="3"/>
       <c r="T9" s="3"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -882,7 +882,7 @@
       <c r="P10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -908,7 +908,7 @@
       <c r="P11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -934,7 +934,7 @@
       <c r="P12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -960,7 +960,7 @@
       <c r="P13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -986,7 +986,7 @@
       <c r="P14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1012,7 +1012,7 @@
       <c r="P15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1038,7 +1038,7 @@
       <c r="P16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1064,7 +1064,7 @@
       <c r="P17" s="3"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1090,7 +1090,7 @@
       <c r="P18" s="3"/>
       <c r="T18" s="3"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1116,22 +1116,22 @@
       <c r="P19" s="3"/>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="L20" s="3"/>
       <c r="P20" s="3"/>
       <c r="T20" s="3"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="L21" s="3"/>
       <c r="P21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="L22" s="3"/>
       <c r="P22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1150,12 +1150,12 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2001</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2002</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2003</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>2.76</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2004</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2005</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>3.19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2006</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>3.08</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2007</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2008</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2009</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2010</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>3.26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2011</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>3.57</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2012</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2013</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>3.46</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2014</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>3.69</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2015</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2016</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2017</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>3.23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2018</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2020</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>3.32</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2021</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>3.55</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2022</v>
       </c>
@@ -1352,12 +1352,12 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2009</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>5449.7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2010</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>6290.9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2011</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>6784.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2012</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>7463.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2013</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>8484.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2014</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>9589.0010000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2015</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>11375.2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2016</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>12806.9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2017</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>15321</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>16788.8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2019</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>17981.7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2020</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>15823.1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2021</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>20321.900000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2022</v>
       </c>
@@ -1490,13 +1490,13 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>26</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>2000</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <v>2001</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>2002</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>2003</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>2004</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>2005</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>2006</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>2007</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>2008</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="9">
         <v>2009</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>2010</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>2011</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>2012</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>2013</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>2014</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>2015</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>2016</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>2017</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>2018</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
         <v>2019</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <v>2020</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="9">
         <v>2021</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <v>2022</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2023</v>
       </c>
@@ -1709,13 +1709,13 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>26</v>
       </c>
@@ -1724,7 +1724,7 @@
       </c>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>2001</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <v>2002</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>5.13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>2003</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>2004</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>2005</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>2006</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>5.95</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>2007</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>8.67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>2008</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>12.32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>2009</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>2010</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>10.49</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>2011</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>13.19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>2012</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>14.62</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>2013</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>13.86</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>2014</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>12.29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>2015</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>9.42</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>2016</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>9.8800000000000008</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>2017</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>9.7799999999999994</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>2018</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>9.35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>2019</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>8.93</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>2020</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>9.5299999999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>2021</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>13.69</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>2022</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>2023</v>
       </c>
@@ -1921,13 +1921,13 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>26</v>
       </c>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>2001</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="12">
         <v>2002</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>2003</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>2004</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>2005</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>2006</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>2007</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>2008</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>2009</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>2010</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>2011</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>2012</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>2013</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>2014</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>2015</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>2016</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>2017</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>2018</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>2019</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>2020</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>2021</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>2022</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>2023</v>
       </c>

</xml_diff>